<commit_message>
Add the third condition
</commit_message>
<xml_diff>
--- a/script/Max/cond/cb.xlsx
+++ b/script/Max/cond/cb.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsukotominaga/OneDrive - Central European University/Project/TeachingPiano/script/Max/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsukotominaga/OneDrive - Central European University/Project/ExpertPiano/script/Max/cond/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{18254B6C-6F0E-484E-BE8D-5C91567D5B9D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{70790A5E-329B-584B-B15B-44A1D8FB927F}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="13_ncr:1_{18254B6C-6F0E-484E-BE8D-5C91567D5B9D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{99C06ACB-ECBA-1647-BD51-704C6961024D}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="840" windowWidth="28040" windowHeight="17440" xr2:uid="{52DF1984-8799-084D-A002-69ECD2D6256B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="24">
   <si>
     <t>;</t>
   </si>
@@ -76,6 +76,27 @@
   </si>
   <si>
     <t>stim_t</t>
+  </si>
+  <si>
+    <t>stim_d</t>
+  </si>
+  <si>
+    <t>dynamics</t>
+  </si>
+  <si>
+    <t>thirdSkill</t>
+  </si>
+  <si>
+    <t>inst_1</t>
+  </si>
+  <si>
+    <t>inst_2</t>
+  </si>
+  <si>
+    <t>inst_t</t>
+  </si>
+  <si>
+    <t>inst_p</t>
   </si>
 </sst>
 </file>
@@ -427,15 +448,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F79E29-5F9D-CD42-974F-D0505AEE028B}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="X10" sqref="N2:X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -446,40 +467,64 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" t="s">
+      <c r="T1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="W1" t="s">
         <v>8</v>
       </c>
+      <c r="X1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -490,53 +535,81 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>1</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>0</v>
       </c>
-      <c r="J2" t="str">
-        <f>CONCATENATE(A2,H2)</f>
+      <c r="N2" t="str">
+        <f>CONCATENATE(A2,L2)</f>
         <v>1,</v>
       </c>
-      <c r="K2" t="str">
+      <c r="O2" t="str">
         <f>B2</f>
         <v>Teaching</v>
       </c>
-      <c r="L2" t="str">
+      <c r="P2" t="str">
         <f>C2</f>
         <v>Performing</v>
       </c>
-      <c r="M2" t="str">
+      <c r="Q2" t="str">
         <f>D2</f>
+        <v>inst_t</v>
+      </c>
+      <c r="R2" t="str">
+        <f>E2</f>
+        <v>inst_p</v>
+      </c>
+      <c r="S2" t="str">
+        <f>F2</f>
         <v>articulation</v>
       </c>
-      <c r="N2" t="str">
-        <f>E2</f>
+      <c r="T2" t="str">
+        <f t="shared" ref="T2:U2" si="0">G2</f>
+        <v>dynamics</v>
+      </c>
+      <c r="U2" t="str">
+        <f t="shared" si="0"/>
         <v>tempoChange</v>
       </c>
-      <c r="O2" t="str">
-        <f>F2</f>
+      <c r="V2" t="str">
+        <f>I2</f>
         <v>stim_a</v>
       </c>
-      <c r="P2" t="str">
-        <f>CONCATENATE(G2,I2)</f>
+      <c r="W2" t="str">
+        <f>J2</f>
+        <v>stim_d</v>
+      </c>
+      <c r="X2" t="str">
+        <f>CONCATENATE(K2,M2)</f>
         <v>stim_t;</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -547,53 +620,81 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>0</v>
       </c>
-      <c r="J3" t="str">
-        <f t="shared" ref="J3:J9" si="0">CONCATENATE(A3,H3)</f>
+      <c r="N3" t="str">
+        <f>CONCATENATE(A3,L3)</f>
         <v>2,</v>
       </c>
-      <c r="K3" t="str">
-        <f t="shared" ref="K3:K9" si="1">B3</f>
+      <c r="O3" t="str">
+        <f>B3</f>
         <v>Performing</v>
       </c>
-      <c r="L3" t="str">
-        <f t="shared" ref="L3:L9" si="2">C3</f>
+      <c r="P3" t="str">
+        <f>C3</f>
         <v>Teaching</v>
       </c>
-      <c r="M3" t="str">
-        <f t="shared" ref="M3:M9" si="3">D3</f>
+      <c r="Q3" t="str">
+        <f t="shared" ref="Q3:Q10" si="1">D3</f>
+        <v>inst_p</v>
+      </c>
+      <c r="R3" t="str">
+        <f t="shared" ref="R3:R10" si="2">E3</f>
+        <v>inst_t</v>
+      </c>
+      <c r="S3" t="str">
+        <f t="shared" ref="S3:S9" si="3">F3</f>
+        <v>dynamics</v>
+      </c>
+      <c r="T3" t="str">
+        <f t="shared" ref="T3:T10" si="4">G3</f>
+        <v>tempoChange</v>
+      </c>
+      <c r="U3" t="str">
+        <f t="shared" ref="U3:U10" si="5">H3</f>
         <v>articulation</v>
       </c>
-      <c r="N3" t="str">
-        <f t="shared" ref="N3:N9" si="4">E3</f>
-        <v>tempoChange</v>
-      </c>
-      <c r="O3" t="str">
-        <f t="shared" ref="O3:O9" si="5">F3</f>
-        <v>stim_a</v>
-      </c>
-      <c r="P3" t="str">
-        <f t="shared" ref="P3:P9" si="6">CONCATENATE(G3,I3)</f>
-        <v>stim_t;</v>
+      <c r="V3" t="str">
+        <f t="shared" ref="V3:V10" si="6">I3</f>
+        <v>stim_d</v>
+      </c>
+      <c r="W3" t="str">
+        <f t="shared" ref="W3:W10" si="7">J3</f>
+        <v>stim_t</v>
+      </c>
+      <c r="X3" t="str">
+        <f t="shared" ref="X3:X10" si="8">CONCATENATE(K3,M3)</f>
+        <v>stim_a;</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -604,335 +705,588 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" t="str">
+        <f>CONCATENATE(A4,L4)</f>
+        <v>3,</v>
+      </c>
+      <c r="O4" t="str">
+        <f>B4</f>
+        <v>Teaching</v>
+      </c>
+      <c r="P4" t="str">
+        <f>C4</f>
+        <v>Performing</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" si="1"/>
+        <v>inst_t</v>
+      </c>
+      <c r="R4" t="str">
+        <f t="shared" si="2"/>
+        <v>inst_p</v>
+      </c>
+      <c r="S4" t="str">
+        <f t="shared" si="3"/>
+        <v>tempoChange</v>
+      </c>
+      <c r="T4" t="str">
+        <f t="shared" si="4"/>
+        <v>articulation</v>
+      </c>
+      <c r="U4" t="str">
+        <f t="shared" si="5"/>
+        <v>dynamics</v>
+      </c>
+      <c r="V4" t="str">
+        <f t="shared" si="6"/>
+        <v>stim_t</v>
+      </c>
+      <c r="W4" t="str">
+        <f t="shared" si="7"/>
+        <v>stim_a</v>
+      </c>
+      <c r="X4" t="str">
+        <f t="shared" si="8"/>
+        <v>stim_d;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I5" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s">
         <v>16</v>
       </c>
-      <c r="H4" t="s">
+      <c r="L5" t="s">
         <v>1</v>
       </c>
-      <c r="I4" t="s">
+      <c r="M5" t="s">
         <v>0</v>
       </c>
-      <c r="J4" t="str">
-        <f t="shared" si="0"/>
-        <v>3,</v>
-      </c>
-      <c r="K4" t="str">
+      <c r="N5" t="str">
+        <f>CONCATENATE(A5,L5)</f>
+        <v>4,</v>
+      </c>
+      <c r="O5" t="str">
+        <f>B5</f>
+        <v>Performing</v>
+      </c>
+      <c r="P5" t="str">
+        <f>C5</f>
+        <v>Teaching</v>
+      </c>
+      <c r="Q5" t="str">
         <f t="shared" si="1"/>
-        <v>Teaching</v>
-      </c>
-      <c r="L4" t="str">
+        <v>inst_p</v>
+      </c>
+      <c r="R5" t="str">
         <f t="shared" si="2"/>
-        <v>Performing</v>
-      </c>
-      <c r="M4" t="str">
+        <v>inst_t</v>
+      </c>
+      <c r="S5" t="str">
         <f t="shared" si="3"/>
         <v>articulation</v>
       </c>
-      <c r="N4" t="str">
+      <c r="T5" t="str">
+        <f t="shared" si="4"/>
+        <v>dynamics</v>
+      </c>
+      <c r="U5" t="str">
+        <f t="shared" si="5"/>
+        <v>tempoChange</v>
+      </c>
+      <c r="V5" t="str">
+        <f t="shared" si="6"/>
+        <v>stim_a</v>
+      </c>
+      <c r="W5" t="str">
+        <f t="shared" si="7"/>
+        <v>stim_d</v>
+      </c>
+      <c r="X5" t="str">
+        <f t="shared" si="8"/>
+        <v>stim_t;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" t="str">
+        <f>CONCATENATE(A6,L6)</f>
+        <v>5,</v>
+      </c>
+      <c r="O6" t="str">
+        <f>B6</f>
+        <v>Teaching</v>
+      </c>
+      <c r="P6" t="str">
+        <f>C6</f>
+        <v>Performing</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="1"/>
+        <v>inst_t</v>
+      </c>
+      <c r="R6" t="str">
+        <f t="shared" si="2"/>
+        <v>inst_p</v>
+      </c>
+      <c r="S6" t="str">
+        <f t="shared" si="3"/>
+        <v>dynamics</v>
+      </c>
+      <c r="T6" t="str">
         <f t="shared" si="4"/>
         <v>tempoChange</v>
       </c>
-      <c r="O4" t="str">
+      <c r="U6" t="str">
         <f t="shared" si="5"/>
+        <v>articulation</v>
+      </c>
+      <c r="V6" t="str">
+        <f t="shared" si="6"/>
+        <v>stim_d</v>
+      </c>
+      <c r="W6" t="str">
+        <f t="shared" si="7"/>
+        <v>stim_t</v>
+      </c>
+      <c r="X6" t="str">
+        <f t="shared" si="8"/>
+        <v>stim_a;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" t="str">
+        <f>CONCATENATE(A7,L7)</f>
+        <v>6,</v>
+      </c>
+      <c r="O7" t="str">
+        <f>B7</f>
+        <v>Performing</v>
+      </c>
+      <c r="P7" t="str">
+        <f>C7</f>
+        <v>Teaching</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="1"/>
+        <v>inst_p</v>
+      </c>
+      <c r="R7" t="str">
+        <f t="shared" si="2"/>
+        <v>inst_t</v>
+      </c>
+      <c r="S7" t="str">
+        <f t="shared" si="3"/>
+        <v>tempoChange</v>
+      </c>
+      <c r="T7" t="str">
+        <f t="shared" si="4"/>
+        <v>articulation</v>
+      </c>
+      <c r="U7" t="str">
+        <f t="shared" si="5"/>
+        <v>dynamics</v>
+      </c>
+      <c r="V7" t="str">
+        <f t="shared" si="6"/>
+        <v>stim_t</v>
+      </c>
+      <c r="W7" t="str">
+        <f t="shared" si="7"/>
         <v>stim_a</v>
       </c>
-      <c r="P4" t="str">
-        <f t="shared" si="6"/>
-        <v>stim_t;</v>
+      <c r="X7" t="str">
+        <f t="shared" si="8"/>
+        <v>stim_d;</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I8" t="s">
         <v>15</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="s">
+      <c r="L8" t="s">
         <v>1</v>
       </c>
-      <c r="I5" t="s">
+      <c r="M8" t="s">
         <v>0</v>
       </c>
-      <c r="J5" t="str">
-        <f t="shared" si="0"/>
-        <v>4,</v>
-      </c>
-      <c r="K5" t="str">
+      <c r="N8" t="str">
+        <f>CONCATENATE(A8,L8)</f>
+        <v>7,</v>
+      </c>
+      <c r="O8" t="str">
+        <f>B8</f>
+        <v>Teaching</v>
+      </c>
+      <c r="P8" t="str">
+        <f>C8</f>
+        <v>Performing</v>
+      </c>
+      <c r="Q8" t="str">
         <f t="shared" si="1"/>
-        <v>Performing</v>
-      </c>
-      <c r="L5" t="str">
+        <v>inst_t</v>
+      </c>
+      <c r="R8" t="str">
         <f t="shared" si="2"/>
-        <v>Teaching</v>
-      </c>
-      <c r="M5" t="str">
+        <v>inst_p</v>
+      </c>
+      <c r="S8" t="str">
         <f t="shared" si="3"/>
         <v>articulation</v>
       </c>
-      <c r="N5" t="str">
+      <c r="T8" t="str">
+        <f t="shared" si="4"/>
+        <v>dynamics</v>
+      </c>
+      <c r="U8" t="str">
+        <f t="shared" si="5"/>
+        <v>tempoChange</v>
+      </c>
+      <c r="V8" t="str">
+        <f t="shared" si="6"/>
+        <v>stim_a</v>
+      </c>
+      <c r="W8" t="str">
+        <f t="shared" si="7"/>
+        <v>stim_d</v>
+      </c>
+      <c r="X8" t="str">
+        <f t="shared" si="8"/>
+        <v>stim_t;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" t="str">
+        <f>CONCATENATE(A9,L9)</f>
+        <v>8,</v>
+      </c>
+      <c r="O9" t="str">
+        <f>B9</f>
+        <v>Performing</v>
+      </c>
+      <c r="P9" t="str">
+        <f>C9</f>
+        <v>Teaching</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="1"/>
+        <v>inst_p</v>
+      </c>
+      <c r="R9" t="str">
+        <f t="shared" si="2"/>
+        <v>inst_t</v>
+      </c>
+      <c r="S9" t="str">
+        <f t="shared" si="3"/>
+        <v>dynamics</v>
+      </c>
+      <c r="T9" t="str">
         <f t="shared" si="4"/>
         <v>tempoChange</v>
       </c>
-      <c r="O5" t="str">
+      <c r="U9" t="str">
         <f t="shared" si="5"/>
-        <v>stim_a</v>
-      </c>
-      <c r="P5" t="str">
+        <v>articulation</v>
+      </c>
+      <c r="V9" t="str">
         <f t="shared" si="6"/>
-        <v>stim_t;</v>
+        <v>stim_d</v>
+      </c>
+      <c r="W9" t="str">
+        <f t="shared" si="7"/>
+        <v>stim_t</v>
+      </c>
+      <c r="X9" t="str">
+        <f t="shared" si="8"/>
+        <v>stim_a;</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
         <v>3</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G10" t="s">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" t="s">
         <v>16</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J10" t="s">
         <v>15</v>
       </c>
-      <c r="H6" t="s">
+      <c r="K10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" t="s">
         <v>1</v>
       </c>
-      <c r="I6" t="s">
+      <c r="M10" t="s">
         <v>0</v>
       </c>
-      <c r="J6" t="str">
-        <f t="shared" si="0"/>
-        <v>5,</v>
-      </c>
-      <c r="K6" t="str">
+      <c r="N10" t="str">
+        <f>CONCATENATE(A10,L10)</f>
+        <v>9,</v>
+      </c>
+      <c r="O10" t="str">
+        <f>B10</f>
+        <v>Teaching</v>
+      </c>
+      <c r="P10" t="str">
+        <f>C10</f>
+        <v>Performing</v>
+      </c>
+      <c r="Q10" t="str">
         <f t="shared" si="1"/>
-        <v>Teaching</v>
-      </c>
-      <c r="L6" t="str">
+        <v>inst_t</v>
+      </c>
+      <c r="R10" t="str">
         <f t="shared" si="2"/>
-        <v>Performing</v>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" si="3"/>
+        <v>inst_p</v>
+      </c>
+      <c r="S10" t="str">
+        <f>F10</f>
         <v>tempoChange</v>
       </c>
-      <c r="N6" t="str">
+      <c r="T10" t="str">
         <f t="shared" si="4"/>
         <v>articulation</v>
       </c>
-      <c r="O6" t="str">
+      <c r="U10" t="str">
         <f t="shared" si="5"/>
+        <v>dynamics</v>
+      </c>
+      <c r="V10" t="str">
+        <f t="shared" si="6"/>
         <v>stim_t</v>
       </c>
-      <c r="P6" t="str">
-        <f t="shared" si="6"/>
-        <v>stim_a;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" si="0"/>
-        <v>6,</v>
-      </c>
-      <c r="K7" t="str">
-        <f t="shared" si="1"/>
-        <v>Performing</v>
-      </c>
-      <c r="L7" t="str">
-        <f t="shared" si="2"/>
-        <v>Teaching</v>
-      </c>
-      <c r="M7" t="str">
-        <f t="shared" si="3"/>
-        <v>tempoChange</v>
-      </c>
-      <c r="N7" t="str">
-        <f t="shared" si="4"/>
-        <v>articulation</v>
-      </c>
-      <c r="O7" t="str">
-        <f t="shared" si="5"/>
-        <v>stim_t</v>
-      </c>
-      <c r="P7" t="str">
-        <f t="shared" si="6"/>
-        <v>stim_a;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" si="0"/>
-        <v>7,</v>
-      </c>
-      <c r="K8" t="str">
-        <f t="shared" si="1"/>
-        <v>Teaching</v>
-      </c>
-      <c r="L8" t="str">
-        <f t="shared" si="2"/>
-        <v>Performing</v>
-      </c>
-      <c r="M8" t="str">
-        <f t="shared" si="3"/>
-        <v>tempoChange</v>
-      </c>
-      <c r="N8" t="str">
-        <f t="shared" si="4"/>
-        <v>articulation</v>
-      </c>
-      <c r="O8" t="str">
-        <f t="shared" si="5"/>
-        <v>stim_t</v>
-      </c>
-      <c r="P8" t="str">
-        <f t="shared" si="6"/>
-        <v>stim_a;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" t="str">
-        <f t="shared" si="0"/>
-        <v>8,</v>
-      </c>
-      <c r="K9" t="str">
-        <f t="shared" si="1"/>
-        <v>Performing</v>
-      </c>
-      <c r="L9" t="str">
-        <f t="shared" si="2"/>
-        <v>Teaching</v>
-      </c>
-      <c r="M9" t="str">
-        <f t="shared" si="3"/>
-        <v>tempoChange</v>
-      </c>
-      <c r="N9" t="str">
-        <f t="shared" si="4"/>
-        <v>articulation</v>
-      </c>
-      <c r="O9" t="str">
-        <f t="shared" si="5"/>
-        <v>stim_t</v>
-      </c>
-      <c r="P9" t="str">
-        <f t="shared" si="6"/>
-        <v>stim_a;</v>
+      <c r="W10" t="str">
+        <f t="shared" si="7"/>
+        <v>stim_a</v>
+      </c>
+      <c r="X10" t="str">
+        <f t="shared" si="8"/>
+        <v>stim_d;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove the third skill (tempoChange)
</commit_message>
<xml_diff>
--- a/script/Max/cond/cb.xlsx
+++ b/script/Max/cond/cb.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="7160" yWindow="1760" windowWidth="28040" windowHeight="17440"/>
@@ -464,7 +464,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -474,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -575,36 +575,36 @@
         <v>1,</v>
       </c>
       <c r="M2" t="str">
-        <f>B2</f>
+        <f t="shared" ref="M2:T2" si="0">B2</f>
         <v>teaching</v>
       </c>
       <c r="N2" t="str">
-        <f>C2</f>
+        <f t="shared" si="0"/>
         <v>performing</v>
       </c>
       <c r="O2" t="str">
-        <f>D2</f>
+        <f t="shared" si="0"/>
         <v>inst_t</v>
       </c>
       <c r="P2" t="str">
-        <f>E2</f>
+        <f t="shared" si="0"/>
         <v>inst_p</v>
       </c>
       <c r="Q2" t="str">
-        <f>F2</f>
+        <f t="shared" si="0"/>
         <v>articulation</v>
       </c>
       <c r="R2" t="str">
-        <f>G2</f>
+        <f t="shared" si="0"/>
         <v>dynamics</v>
       </c>
       <c r="S2" t="str">
-        <f>H2</f>
+        <f t="shared" si="0"/>
         <v>stim_a</v>
       </c>
       <c r="T2" t="str">
-        <f>I2</f>
-        <v>stim_d</v>
+        <f>CONCATENATE(I2,K2)</f>
+        <v>stim_d;</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -642,40 +642,40 @@
         <v>0</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L11" si="0">CONCATENATE(A3,J3)</f>
+        <f t="shared" ref="L3:L11" si="1">CONCATENATE(A3,J3)</f>
         <v>2,</v>
       </c>
       <c r="M3" t="str">
-        <f t="shared" ref="M3:M11" si="1">B3</f>
+        <f t="shared" ref="M3:M11" si="2">B3</f>
         <v>performing</v>
       </c>
       <c r="N3" t="str">
-        <f t="shared" ref="N3:N11" si="2">C3</f>
+        <f t="shared" ref="N3:N11" si="3">C3</f>
         <v>teaching</v>
       </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O11" si="3">D3</f>
+        <f t="shared" ref="O3:O11" si="4">D3</f>
         <v>inst_p</v>
       </c>
       <c r="P3" t="str">
-        <f t="shared" ref="P3:P11" si="4">E3</f>
+        <f t="shared" ref="P3:P11" si="5">E3</f>
         <v>inst_t</v>
       </c>
       <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q11" si="5">F3</f>
+        <f t="shared" ref="Q3:Q11" si="6">F3</f>
         <v>dynamics</v>
       </c>
       <c r="R3" t="str">
-        <f t="shared" ref="R3:R11" si="6">G3</f>
+        <f t="shared" ref="R3:R11" si="7">G3</f>
         <v>articulation</v>
       </c>
       <c r="S3" t="str">
-        <f t="shared" ref="S3:S11" si="7">H3</f>
+        <f t="shared" ref="S3:S11" si="8">H3</f>
         <v>stim_d</v>
       </c>
       <c r="T3" t="str">
-        <f t="shared" ref="T3:T11" si="8">I3</f>
-        <v>stim_a</v>
+        <f t="shared" ref="T3:T11" si="9">CONCATENATE(I3,K3)</f>
+        <v>stim_a;</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -713,40 +713,40 @@
         <v>0</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3,</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>teaching</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>performing</v>
       </c>
       <c r="O4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>inst_t</v>
       </c>
       <c r="P4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>inst_p</v>
       </c>
       <c r="Q4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>articulation</v>
       </c>
       <c r="R4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>dynamics</v>
       </c>
       <c r="S4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>stim_a</v>
       </c>
       <c r="T4" t="str">
-        <f t="shared" si="8"/>
-        <v>stim_d</v>
+        <f t="shared" si="9"/>
+        <v>stim_d;</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -784,40 +784,40 @@
         <v>0</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4,</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>performing</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>teaching</v>
       </c>
       <c r="O5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>inst_p</v>
       </c>
       <c r="P5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>inst_t</v>
       </c>
       <c r="Q5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>dynamics</v>
       </c>
       <c r="R5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>articulation</v>
       </c>
       <c r="S5" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>stim_d</v>
       </c>
       <c r="T5" t="str">
-        <f t="shared" si="8"/>
-        <v>stim_a</v>
+        <f t="shared" si="9"/>
+        <v>stim_a;</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -855,40 +855,40 @@
         <v>0</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5,</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>teaching</v>
       </c>
       <c r="N6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>performing</v>
       </c>
       <c r="O6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>inst_t</v>
       </c>
       <c r="P6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>inst_p</v>
       </c>
       <c r="Q6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>articulation</v>
       </c>
       <c r="R6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>dynamics</v>
       </c>
       <c r="S6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>stim_a</v>
       </c>
       <c r="T6" t="str">
-        <f t="shared" si="8"/>
-        <v>stim_d</v>
+        <f t="shared" si="9"/>
+        <v>stim_d;</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -926,40 +926,40 @@
         <v>0</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6,</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>performing</v>
       </c>
       <c r="N7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>teaching</v>
       </c>
       <c r="O7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>inst_p</v>
       </c>
       <c r="P7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>inst_t</v>
       </c>
       <c r="Q7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>dynamics</v>
       </c>
       <c r="R7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>articulation</v>
       </c>
       <c r="S7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>stim_d</v>
       </c>
       <c r="T7" t="str">
-        <f t="shared" si="8"/>
-        <v>stim_a</v>
+        <f t="shared" si="9"/>
+        <v>stim_a;</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -997,40 +997,40 @@
         <v>0</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7,</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>teaching</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>performing</v>
       </c>
       <c r="O8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>inst_t</v>
       </c>
       <c r="P8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>inst_p</v>
       </c>
       <c r="Q8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>articulation</v>
       </c>
       <c r="R8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>dynamics</v>
       </c>
       <c r="S8" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>stim_a</v>
       </c>
       <c r="T8" t="str">
-        <f t="shared" si="8"/>
-        <v>stim_d</v>
+        <f t="shared" si="9"/>
+        <v>stim_d;</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -1068,40 +1068,40 @@
         <v>0</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8,</v>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>performing</v>
       </c>
       <c r="N9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>teaching</v>
       </c>
       <c r="O9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>inst_p</v>
       </c>
       <c r="P9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>inst_t</v>
       </c>
       <c r="Q9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>dynamics</v>
       </c>
       <c r="R9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>articulation</v>
       </c>
       <c r="S9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>stim_d</v>
       </c>
       <c r="T9" t="str">
-        <f t="shared" si="8"/>
-        <v>stim_a</v>
+        <f t="shared" si="9"/>
+        <v>stim_a;</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1139,40 +1139,40 @@
         <v>0</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9,</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>teaching</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>performing</v>
       </c>
       <c r="O10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>inst_t</v>
       </c>
       <c r="P10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>inst_p</v>
       </c>
       <c r="Q10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>articulation</v>
       </c>
       <c r="R10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>dynamics</v>
       </c>
       <c r="S10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>stim_a</v>
       </c>
       <c r="T10" t="str">
-        <f t="shared" si="8"/>
-        <v>stim_d</v>
+        <f t="shared" si="9"/>
+        <v>stim_d;</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1210,40 +1210,40 @@
         <v>0</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10,</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>performing</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>teaching</v>
       </c>
       <c r="O11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>inst_p</v>
       </c>
       <c r="P11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>inst_t</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>dynamics</v>
       </c>
       <c r="R11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>articulation</v>
       </c>
       <c r="S11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>stim_d</v>
       </c>
       <c r="T11" t="str">
-        <f t="shared" si="8"/>
-        <v>stim_a</v>
+        <f t="shared" si="9"/>
+        <v>stim_a;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update a counterbalance sheet
</commit_message>
<xml_diff>
--- a/script/Max/cond/cb.xlsx
+++ b/script/Max/cond/cb.xlsx
@@ -133,8 +133,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -149,17 +155,23 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,7 +476,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -475,7 +487,7 @@
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:T11"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -575,7 +587,7 @@
         <v>1,</v>
       </c>
       <c r="M2" t="str">
-        <f t="shared" ref="M2:T2" si="0">B2</f>
+        <f t="shared" ref="M2:S2" si="0">B2</f>
         <v>teaching</v>
       </c>
       <c r="N2" t="str">
@@ -630,10 +642,10 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
         <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
       </c>
       <c r="J3" t="s">
         <v>1</v>
@@ -671,11 +683,11 @@
       </c>
       <c r="S3" t="str">
         <f t="shared" ref="S3:S11" si="8">H3</f>
-        <v>stim_d</v>
+        <v>stim_a</v>
       </c>
       <c r="T3" t="str">
         <f t="shared" ref="T3:T11" si="9">CONCATENATE(I3,K3)</f>
-        <v>stim_a;</v>
+        <v>stim_d;</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -701,10 +713,10 @@
         <v>14</v>
       </c>
       <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
         <v>12</v>
-      </c>
-      <c r="I4" t="s">
-        <v>13</v>
       </c>
       <c r="J4" t="s">
         <v>1</v>
@@ -742,11 +754,11 @@
       </c>
       <c r="S4" t="str">
         <f t="shared" si="8"/>
-        <v>stim_a</v>
+        <v>stim_d</v>
       </c>
       <c r="T4" t="str">
         <f t="shared" si="9"/>
-        <v>stim_d;</v>
+        <v>stim_a;</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -914,10 +926,10 @@
         <v>2</v>
       </c>
       <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" t="s">
         <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>12</v>
       </c>
       <c r="J7" t="s">
         <v>1</v>
@@ -955,11 +967,11 @@
       </c>
       <c r="S7" t="str">
         <f t="shared" si="8"/>
-        <v>stim_d</v>
+        <v>stim_a</v>
       </c>
       <c r="T7" t="str">
         <f t="shared" si="9"/>
-        <v>stim_a;</v>
+        <v>stim_d;</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -985,10 +997,10 @@
         <v>14</v>
       </c>
       <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
         <v>12</v>
-      </c>
-      <c r="I8" t="s">
-        <v>13</v>
       </c>
       <c r="J8" t="s">
         <v>1</v>
@@ -1026,11 +1038,11 @@
       </c>
       <c r="S8" t="str">
         <f t="shared" si="8"/>
-        <v>stim_a</v>
+        <v>stim_d</v>
       </c>
       <c r="T8" t="str">
         <f t="shared" si="9"/>
-        <v>stim_d;</v>
+        <v>stim_a;</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -1198,10 +1210,10 @@
         <v>2</v>
       </c>
       <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" t="s">
         <v>13</v>
-      </c>
-      <c r="I11" t="s">
-        <v>12</v>
       </c>
       <c r="J11" t="s">
         <v>1</v>
@@ -1239,11 +1251,11 @@
       </c>
       <c r="S11" t="str">
         <f t="shared" si="8"/>
-        <v>stim_d</v>
+        <v>stim_a</v>
       </c>
       <c r="T11" t="str">
         <f t="shared" si="9"/>
-        <v>stim_a;</v>
+        <v>stim_d;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct cond (skill names and img names were not corresponded)
</commit_message>
<xml_diff>
--- a/script/Max/cond/cb.xlsx
+++ b/script/Max/cond/cb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsukotominaga/OneDrive - Central European University/Project/expertpiano/script/Max/cond/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_297695AA3A6FA689C6D9BB6F54EBB5FC431D7C89" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{7BD18A95-4E03-944A-92D6-43013DD5B1A2}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_297695AA3A6FA689C6D9BB6F54EBB5FC431D7C89" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{BEDAB7F4-34A9-FE41-8963-4CD0310E24B1}"/>
   <bookViews>
     <workbookView xWindow="5560" yWindow="1760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,10 +666,10 @@
         <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>12</v>
@@ -705,11 +705,11 @@
       </c>
       <c r="Q3" t="str">
         <f t="shared" ref="Q3:Q31" si="6">F3</f>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="R3" t="str">
         <f t="shared" ref="R3:R31" si="7">G3</f>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="S3" t="str">
         <f t="shared" ref="S3:S31" si="8">H3</f>
@@ -737,10 +737,10 @@
         <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>13</v>
@@ -776,11 +776,11 @@
       </c>
       <c r="Q4" t="str">
         <f t="shared" si="6"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="R4" t="str">
         <f t="shared" si="7"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="S4" t="str">
         <f t="shared" si="8"/>
@@ -950,10 +950,10 @@
         <v>17</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>12</v>
@@ -989,11 +989,11 @@
       </c>
       <c r="Q7" t="str">
         <f t="shared" si="6"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="R7" t="str">
         <f t="shared" si="7"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="S7" t="str">
         <f t="shared" si="8"/>
@@ -1021,10 +1021,10 @@
         <v>18</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>13</v>
@@ -1060,11 +1060,11 @@
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="6"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="R8" t="str">
         <f t="shared" si="7"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="S8" t="str">
         <f t="shared" si="8"/>
@@ -1234,10 +1234,10 @@
         <v>17</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>12</v>
@@ -1273,11 +1273,11 @@
       </c>
       <c r="Q11" t="str">
         <f t="shared" si="6"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="R11" t="str">
         <f t="shared" si="7"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="S11" t="str">
         <f t="shared" si="8"/>
@@ -1305,10 +1305,10 @@
         <v>18</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>12</v>
@@ -1344,11 +1344,11 @@
       </c>
       <c r="Q12" t="str">
         <f t="shared" si="6"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" si="7"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="S12" t="str">
         <f t="shared" si="8"/>
@@ -1518,10 +1518,10 @@
         <v>17</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>13</v>
@@ -1557,11 +1557,11 @@
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="6"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" si="7"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="8"/>
@@ -1589,10 +1589,10 @@
         <v>18</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>12</v>
@@ -1628,11 +1628,11 @@
       </c>
       <c r="Q16" t="str">
         <f t="shared" si="6"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" si="7"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="S16" t="str">
         <f t="shared" si="8"/>
@@ -1802,10 +1802,10 @@
         <v>17</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>13</v>
@@ -1841,11 +1841,11 @@
       </c>
       <c r="Q19" t="str">
         <f t="shared" si="6"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="R19" t="str">
         <f t="shared" si="7"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="S19" t="str">
         <f t="shared" si="8"/>
@@ -1873,10 +1873,10 @@
         <v>18</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>12</v>
@@ -1912,11 +1912,11 @@
       </c>
       <c r="Q20" t="str">
         <f t="shared" si="6"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="R20" t="str">
         <f t="shared" si="7"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="S20" t="str">
         <f t="shared" si="8"/>
@@ -2086,10 +2086,10 @@
         <v>17</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>12</v>
@@ -2125,11 +2125,11 @@
       </c>
       <c r="Q23" t="str">
         <f t="shared" si="6"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="R23" t="str">
         <f t="shared" si="7"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="S23" t="str">
         <f t="shared" si="8"/>
@@ -2157,10 +2157,10 @@
         <v>18</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>13</v>
@@ -2196,11 +2196,11 @@
       </c>
       <c r="Q24" t="str">
         <f t="shared" si="6"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="R24" t="str">
         <f t="shared" si="7"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="S24" t="str">
         <f t="shared" si="8"/>
@@ -2370,10 +2370,10 @@
         <v>17</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>12</v>
@@ -2409,11 +2409,11 @@
       </c>
       <c r="Q27" t="str">
         <f t="shared" si="6"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="R27" t="str">
         <f t="shared" si="7"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="S27" t="str">
         <f t="shared" si="8"/>
@@ -2441,10 +2441,10 @@
         <v>18</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>13</v>
@@ -2480,11 +2480,11 @@
       </c>
       <c r="Q28" t="str">
         <f t="shared" si="6"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="R28" t="str">
         <f t="shared" si="7"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="S28" t="str">
         <f t="shared" si="8"/>
@@ -2654,10 +2654,10 @@
         <v>17</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>12</v>
@@ -2693,11 +2693,11 @@
       </c>
       <c r="Q31" t="str">
         <f t="shared" si="6"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="R31" t="str">
         <f t="shared" si="7"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="S31" t="str">
         <f t="shared" si="8"/>

</xml_diff>

<commit_message>
Correct cond (skill names and img names were not corresponded; part2)
</commit_message>
<xml_diff>
--- a/script/Max/cond/cb.xlsx
+++ b/script/Max/cond/cb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsukotominaga/OneDrive - Central European University/Project/expertpiano/script/Max/cond/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_297695AA3A6FA689C6D9BB6F54EBB5FC431D7C89" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{BEDAB7F4-34A9-FE41-8963-4CD0310E24B1}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_297695AA3A6FA689C6D9BB6F54EBB5FC431D7C89" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00AB0A66-541A-454A-B3FC-8C4F30C5514E}"/>
   <bookViews>
     <workbookView xWindow="5560" yWindow="1760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="21">
   <si>
     <t>;</t>
   </si>
@@ -514,10 +514,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T31"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -684,39 +687,39 @@
         <v>0</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L31" si="1">CONCATENATE(A3,J3)</f>
+        <f t="shared" ref="L3:L29" si="1">CONCATENATE(A3,J3)</f>
         <v>2,</v>
       </c>
       <c r="M3" t="str">
-        <f t="shared" ref="M3:M31" si="2">B3</f>
+        <f t="shared" ref="M3:M29" si="2">B3</f>
         <v>performing</v>
       </c>
       <c r="N3" t="str">
-        <f t="shared" ref="N3:N31" si="3">C3</f>
+        <f t="shared" ref="N3:N29" si="3">C3</f>
         <v>teaching</v>
       </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O31" si="4">D3</f>
+        <f t="shared" ref="O3:O29" si="4">D3</f>
         <v>inst_p</v>
       </c>
       <c r="P3" t="str">
-        <f t="shared" ref="P3:P31" si="5">E3</f>
+        <f t="shared" ref="P3:P29" si="5">E3</f>
         <v>inst_t</v>
       </c>
       <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q31" si="6">F3</f>
+        <f t="shared" ref="Q3:Q29" si="6">F3</f>
         <v>articulation</v>
       </c>
       <c r="R3" t="str">
-        <f t="shared" ref="R3:R31" si="7">G3</f>
+        <f t="shared" ref="R3:R29" si="7">G3</f>
         <v>dynamics</v>
       </c>
       <c r="S3" t="str">
-        <f t="shared" ref="S3:S31" si="8">H3</f>
+        <f t="shared" ref="S3:S29" si="8">H3</f>
         <v>stim_a</v>
       </c>
       <c r="T3" t="str">
-        <f t="shared" ref="T3:T31" si="9">CONCATENATE(I3,K3)</f>
+        <f t="shared" ref="T3:T29" si="9">CONCATENATE(I3,K3)</f>
         <v>stim_d;</v>
       </c>
     </row>
@@ -1305,10 +1308,10 @@
         <v>18</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>12</v>
@@ -1344,11 +1347,11 @@
       </c>
       <c r="Q12" t="str">
         <f t="shared" si="6"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" si="7"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="S12" t="str">
         <f t="shared" si="8"/>
@@ -1376,10 +1379,10 @@
         <v>17</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>12</v>
@@ -1415,11 +1418,11 @@
       </c>
       <c r="Q13" t="str">
         <f t="shared" si="6"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="R13" t="str">
         <f t="shared" si="7"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="S13" t="str">
         <f t="shared" si="8"/>
@@ -1447,10 +1450,10 @@
         <v>18</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>13</v>
@@ -1486,11 +1489,11 @@
       </c>
       <c r="Q14" t="str">
         <f t="shared" si="6"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="R14" t="str">
         <f t="shared" si="7"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="S14" t="str">
         <f t="shared" si="8"/>
@@ -1518,10 +1521,10 @@
         <v>17</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>13</v>
@@ -1557,11 +1560,11 @@
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="6"/>
-        <v>articulation</v>
+        <v>dynamics</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" si="7"/>
-        <v>dynamics</v>
+        <v>articulation</v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="8"/>
@@ -1595,10 +1598,10 @@
         <v>2</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J16" t="s">
         <v>1</v>
@@ -1636,11 +1639,11 @@
       </c>
       <c r="S16" t="str">
         <f t="shared" si="8"/>
-        <v>stim_a</v>
+        <v>stim_d</v>
       </c>
       <c r="T16" t="str">
         <f t="shared" si="9"/>
-        <v>stim_d;</v>
+        <v>stim_a;</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
@@ -1666,10 +1669,10 @@
         <v>2</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J17" t="s">
         <v>1</v>
@@ -1707,11 +1710,11 @@
       </c>
       <c r="S17" t="str">
         <f t="shared" si="8"/>
-        <v>stim_a</v>
+        <v>stim_d</v>
       </c>
       <c r="T17" t="str">
         <f t="shared" si="9"/>
-        <v>stim_d;</v>
+        <v>stim_a;</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
@@ -1737,10 +1740,10 @@
         <v>14</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J18" t="s">
         <v>1</v>
@@ -1778,11 +1781,11 @@
       </c>
       <c r="S18" t="str">
         <f t="shared" si="8"/>
-        <v>stim_d</v>
+        <v>stim_a</v>
       </c>
       <c r="T18" t="str">
         <f t="shared" si="9"/>
-        <v>stim_a;</v>
+        <v>stim_d;</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
@@ -1808,10 +1811,10 @@
         <v>14</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J19" t="s">
         <v>1</v>
@@ -1849,11 +1852,11 @@
       </c>
       <c r="S19" t="str">
         <f t="shared" si="8"/>
-        <v>stim_d</v>
+        <v>stim_a</v>
       </c>
       <c r="T19" t="str">
         <f t="shared" si="9"/>
-        <v>stim_a;</v>
+        <v>stim_d;</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
@@ -1879,10 +1882,10 @@
         <v>2</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J20" t="s">
         <v>1</v>
@@ -1920,11 +1923,11 @@
       </c>
       <c r="S20" t="str">
         <f t="shared" si="8"/>
-        <v>stim_a</v>
+        <v>stim_d</v>
       </c>
       <c r="T20" t="str">
         <f t="shared" si="9"/>
-        <v>stim_d;</v>
+        <v>stim_a;</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
@@ -1950,10 +1953,10 @@
         <v>2</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J21" t="s">
         <v>1</v>
@@ -1991,11 +1994,11 @@
       </c>
       <c r="S21" t="str">
         <f t="shared" si="8"/>
-        <v>stim_a</v>
+        <v>stim_d</v>
       </c>
       <c r="T21" t="str">
         <f t="shared" si="9"/>
-        <v>stim_d;</v>
+        <v>stim_a;</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
@@ -2566,151 +2569,9 @@
         <v>stim_a;</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J30" t="s">
-        <v>1</v>
-      </c>
-      <c r="K30" t="s">
-        <v>0</v>
-      </c>
-      <c r="L30" t="str">
-        <f t="shared" si="1"/>
-        <v>29,</v>
-      </c>
-      <c r="M30" t="str">
-        <f t="shared" si="2"/>
-        <v>teaching</v>
-      </c>
-      <c r="N30" t="str">
-        <f t="shared" si="3"/>
-        <v>performing</v>
-      </c>
-      <c r="O30" t="str">
-        <f t="shared" si="4"/>
-        <v>inst_t</v>
-      </c>
-      <c r="P30" t="str">
-        <f t="shared" si="5"/>
-        <v>inst_p</v>
-      </c>
-      <c r="Q30" t="str">
-        <f t="shared" si="6"/>
-        <v>articulation</v>
-      </c>
-      <c r="R30" t="str">
-        <f t="shared" si="7"/>
-        <v>dynamics</v>
-      </c>
-      <c r="S30" t="str">
-        <f t="shared" si="8"/>
-        <v>stim_a</v>
-      </c>
-      <c r="T30" t="str">
-        <f t="shared" si="9"/>
-        <v>stim_d;</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J31" t="s">
-        <v>1</v>
-      </c>
-      <c r="K31" t="s">
-        <v>0</v>
-      </c>
-      <c r="L31" t="str">
-        <f t="shared" si="1"/>
-        <v>30,</v>
-      </c>
-      <c r="M31" t="str">
-        <f t="shared" si="2"/>
-        <v>performing</v>
-      </c>
-      <c r="N31" t="str">
-        <f t="shared" si="3"/>
-        <v>teaching</v>
-      </c>
-      <c r="O31" t="str">
-        <f t="shared" si="4"/>
-        <v>inst_p</v>
-      </c>
-      <c r="P31" t="str">
-        <f t="shared" si="5"/>
-        <v>inst_t</v>
-      </c>
-      <c r="Q31" t="str">
-        <f t="shared" si="6"/>
-        <v>articulation</v>
-      </c>
-      <c r="R31" t="str">
-        <f t="shared" si="7"/>
-        <v>dynamics</v>
-      </c>
-      <c r="S31" t="str">
-        <f t="shared" si="8"/>
-        <v>stim_a</v>
-      </c>
-      <c r="T31" t="str">
-        <f t="shared" si="9"/>
-        <v>stim_d;</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="84" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Update cb files (up to 40 subjects)
</commit_message>
<xml_diff>
--- a/script/Max/cond/cb.xlsx
+++ b/script/Max/cond/cb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsukotominaga/OneDrive - Central European University/Project/expertpiano/script/Max/cond/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="11_297695AA3A6FA689C6D9BB6F54EBB5FC431D7C89" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{9124124E-B240-884E-BB9B-C21C4A776966}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="11_297695AA3A6FA689C6D9BB6F54EBB5FC431D7C89" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{2983D57D-0D72-2B44-B7D2-0AD8370E6863}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="1340" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="21">
   <si>
     <t>;</t>
   </si>
@@ -518,10 +518,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T31"/>
+  <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T31" sqref="L1:T31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I41" sqref="A1:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2709,6 +2709,716 @@
       </c>
       <c r="T31" t="str">
         <f t="shared" si="18"/>
+        <v>stim_a;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" t="s">
+        <v>1</v>
+      </c>
+      <c r="K32" t="s">
+        <v>0</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" ref="L32:L41" si="19">CONCATENATE(A32,J32)</f>
+        <v>31,</v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" ref="M32:M41" si="20">B32</f>
+        <v>teaching</v>
+      </c>
+      <c r="N32" t="str">
+        <f t="shared" ref="N32:N41" si="21">C32</f>
+        <v>performing</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" ref="O32:O41" si="22">D32</f>
+        <v>inst_t</v>
+      </c>
+      <c r="P32" t="str">
+        <f t="shared" ref="P32:P41" si="23">E32</f>
+        <v>inst_p</v>
+      </c>
+      <c r="Q32" t="str">
+        <f t="shared" ref="Q32:Q41" si="24">F32</f>
+        <v>articulation</v>
+      </c>
+      <c r="R32" t="str">
+        <f t="shared" ref="R32:R41" si="25">G32</f>
+        <v>dynamics</v>
+      </c>
+      <c r="S32" t="str">
+        <f t="shared" ref="S32:S41" si="26">H32</f>
+        <v>stim_a</v>
+      </c>
+      <c r="T32" t="str">
+        <f t="shared" ref="T32:T41" si="27">CONCATENATE(I32,K32)</f>
+        <v>stim_d;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J33" t="s">
+        <v>1</v>
+      </c>
+      <c r="K33" t="s">
+        <v>0</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="19"/>
+        <v>32,</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="20"/>
+        <v>teaching</v>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="21"/>
+        <v>performing</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="22"/>
+        <v>inst_t</v>
+      </c>
+      <c r="P33" t="str">
+        <f t="shared" si="23"/>
+        <v>inst_p</v>
+      </c>
+      <c r="Q33" t="str">
+        <f t="shared" si="24"/>
+        <v>dynamics</v>
+      </c>
+      <c r="R33" t="str">
+        <f t="shared" si="25"/>
+        <v>articulation</v>
+      </c>
+      <c r="S33" t="str">
+        <f t="shared" si="26"/>
+        <v>stim_d</v>
+      </c>
+      <c r="T33" t="str">
+        <f t="shared" si="27"/>
+        <v>stim_a;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J34" t="s">
+        <v>1</v>
+      </c>
+      <c r="K34" t="s">
+        <v>0</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="19"/>
+        <v>33,</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="20"/>
+        <v>performing</v>
+      </c>
+      <c r="N34" t="str">
+        <f t="shared" si="21"/>
+        <v>teaching</v>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" si="22"/>
+        <v>inst_p</v>
+      </c>
+      <c r="P34" t="str">
+        <f t="shared" si="23"/>
+        <v>inst_t</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" si="24"/>
+        <v>articulation</v>
+      </c>
+      <c r="R34" t="str">
+        <f t="shared" si="25"/>
+        <v>dynamics</v>
+      </c>
+      <c r="S34" t="str">
+        <f t="shared" si="26"/>
+        <v>stim_a</v>
+      </c>
+      <c r="T34" t="str">
+        <f t="shared" si="27"/>
+        <v>stim_d;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J35" t="s">
+        <v>1</v>
+      </c>
+      <c r="K35" t="s">
+        <v>0</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="19"/>
+        <v>34,</v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" si="20"/>
+        <v>teaching</v>
+      </c>
+      <c r="N35" t="str">
+        <f t="shared" si="21"/>
+        <v>performing</v>
+      </c>
+      <c r="O35" t="str">
+        <f t="shared" si="22"/>
+        <v>inst_t</v>
+      </c>
+      <c r="P35" t="str">
+        <f t="shared" si="23"/>
+        <v>inst_p</v>
+      </c>
+      <c r="Q35" t="str">
+        <f t="shared" si="24"/>
+        <v>articulation</v>
+      </c>
+      <c r="R35" t="str">
+        <f t="shared" si="25"/>
+        <v>dynamics</v>
+      </c>
+      <c r="S35" t="str">
+        <f t="shared" si="26"/>
+        <v>stim_a</v>
+      </c>
+      <c r="T35" t="str">
+        <f t="shared" si="27"/>
+        <v>stim_d;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J36" t="s">
+        <v>1</v>
+      </c>
+      <c r="K36" t="s">
+        <v>0</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="19"/>
+        <v>35,</v>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" si="20"/>
+        <v>teaching</v>
+      </c>
+      <c r="N36" t="str">
+        <f t="shared" si="21"/>
+        <v>performing</v>
+      </c>
+      <c r="O36" t="str">
+        <f t="shared" si="22"/>
+        <v>inst_t</v>
+      </c>
+      <c r="P36" t="str">
+        <f t="shared" si="23"/>
+        <v>inst_p</v>
+      </c>
+      <c r="Q36" t="str">
+        <f t="shared" si="24"/>
+        <v>dynamics</v>
+      </c>
+      <c r="R36" t="str">
+        <f t="shared" si="25"/>
+        <v>articulation</v>
+      </c>
+      <c r="S36" t="str">
+        <f t="shared" si="26"/>
+        <v>stim_d</v>
+      </c>
+      <c r="T36" t="str">
+        <f t="shared" si="27"/>
+        <v>stim_a;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J37" t="s">
+        <v>1</v>
+      </c>
+      <c r="K37" t="s">
+        <v>0</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="19"/>
+        <v>36,</v>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" si="20"/>
+        <v>performing</v>
+      </c>
+      <c r="N37" t="str">
+        <f t="shared" si="21"/>
+        <v>teaching</v>
+      </c>
+      <c r="O37" t="str">
+        <f t="shared" si="22"/>
+        <v>inst_p</v>
+      </c>
+      <c r="P37" t="str">
+        <f t="shared" si="23"/>
+        <v>inst_t</v>
+      </c>
+      <c r="Q37" t="str">
+        <f t="shared" si="24"/>
+        <v>articulation</v>
+      </c>
+      <c r="R37" t="str">
+        <f t="shared" si="25"/>
+        <v>dynamics</v>
+      </c>
+      <c r="S37" t="str">
+        <f t="shared" si="26"/>
+        <v>stim_a</v>
+      </c>
+      <c r="T37" t="str">
+        <f t="shared" si="27"/>
+        <v>stim_d;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J38" t="s">
+        <v>1</v>
+      </c>
+      <c r="K38" t="s">
+        <v>0</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="19"/>
+        <v>37,</v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" si="20"/>
+        <v>teaching</v>
+      </c>
+      <c r="N38" t="str">
+        <f t="shared" si="21"/>
+        <v>performing</v>
+      </c>
+      <c r="O38" t="str">
+        <f t="shared" si="22"/>
+        <v>inst_t</v>
+      </c>
+      <c r="P38" t="str">
+        <f t="shared" si="23"/>
+        <v>inst_p</v>
+      </c>
+      <c r="Q38" t="str">
+        <f t="shared" si="24"/>
+        <v>articulation</v>
+      </c>
+      <c r="R38" t="str">
+        <f t="shared" si="25"/>
+        <v>dynamics</v>
+      </c>
+      <c r="S38" t="str">
+        <f t="shared" si="26"/>
+        <v>stim_a</v>
+      </c>
+      <c r="T38" t="str">
+        <f t="shared" si="27"/>
+        <v>stim_d;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J39" t="s">
+        <v>1</v>
+      </c>
+      <c r="K39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="19"/>
+        <v>38,</v>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" si="20"/>
+        <v>performing</v>
+      </c>
+      <c r="N39" t="str">
+        <f t="shared" si="21"/>
+        <v>teaching</v>
+      </c>
+      <c r="O39" t="str">
+        <f t="shared" si="22"/>
+        <v>inst_p</v>
+      </c>
+      <c r="P39" t="str">
+        <f t="shared" si="23"/>
+        <v>inst_t</v>
+      </c>
+      <c r="Q39" t="str">
+        <f t="shared" si="24"/>
+        <v>articulation</v>
+      </c>
+      <c r="R39" t="str">
+        <f t="shared" si="25"/>
+        <v>dynamics</v>
+      </c>
+      <c r="S39" t="str">
+        <f t="shared" si="26"/>
+        <v>stim_a</v>
+      </c>
+      <c r="T39" t="str">
+        <f t="shared" si="27"/>
+        <v>stim_d;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J40" t="s">
+        <v>1</v>
+      </c>
+      <c r="K40" t="s">
+        <v>0</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="19"/>
+        <v>39,</v>
+      </c>
+      <c r="M40" t="str">
+        <f t="shared" si="20"/>
+        <v>teaching</v>
+      </c>
+      <c r="N40" t="str">
+        <f t="shared" si="21"/>
+        <v>performing</v>
+      </c>
+      <c r="O40" t="str">
+        <f t="shared" si="22"/>
+        <v>inst_t</v>
+      </c>
+      <c r="P40" t="str">
+        <f t="shared" si="23"/>
+        <v>inst_p</v>
+      </c>
+      <c r="Q40" t="str">
+        <f t="shared" si="24"/>
+        <v>dynamics</v>
+      </c>
+      <c r="R40" t="str">
+        <f t="shared" si="25"/>
+        <v>articulation</v>
+      </c>
+      <c r="S40" t="str">
+        <f t="shared" si="26"/>
+        <v>stim_d</v>
+      </c>
+      <c r="T40" t="str">
+        <f t="shared" si="27"/>
+        <v>stim_a;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J41" t="s">
+        <v>1</v>
+      </c>
+      <c r="K41" t="s">
+        <v>0</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="19"/>
+        <v>40,</v>
+      </c>
+      <c r="M41" t="str">
+        <f t="shared" si="20"/>
+        <v>performing</v>
+      </c>
+      <c r="N41" t="str">
+        <f t="shared" si="21"/>
+        <v>teaching</v>
+      </c>
+      <c r="O41" t="str">
+        <f t="shared" si="22"/>
+        <v>inst_p</v>
+      </c>
+      <c r="P41" t="str">
+        <f t="shared" si="23"/>
+        <v>inst_t</v>
+      </c>
+      <c r="Q41" t="str">
+        <f t="shared" si="24"/>
+        <v>dynamics</v>
+      </c>
+      <c r="R41" t="str">
+        <f t="shared" si="25"/>
+        <v>articulation</v>
+      </c>
+      <c r="S41" t="str">
+        <f t="shared" si="26"/>
+        <v>stim_d</v>
+      </c>
+      <c r="T41" t="str">
+        <f t="shared" si="27"/>
         <v>stim_a;</v>
       </c>
     </row>

</xml_diff>